<commit_message>
Corretto lista parti sul componente DC/DC 9V
</commit_message>
<xml_diff>
--- a/ESECUTIVI/LP22-304-1.xlsx
+++ b/ESECUTIVI/LP22-304-1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Utenti\00.Lavori in corso\METALTRONICA\22-304-1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco\Documents\Data\Progetti-GIT\HW\PCB-22-304\ESECUTIVI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{CCBA1402-7E34-4548-9DD6-7F0C773B3B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8A50BB-7EF1-442D-A730-F3B5716E2A05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="22-304-1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="290">
   <si>
     <t>Pos.</t>
   </si>
@@ -802,24 +802,12 @@
     <t>U8</t>
   </si>
   <si>
-    <t>DC/DC 5V 1A</t>
-  </si>
-  <si>
     <t>P78E09-1000</t>
   </si>
   <si>
-    <t>P78E05-1000</t>
-  </si>
-  <si>
-    <t>M: 490-P78E05-1000</t>
-  </si>
-  <si>
     <t>TRACO POWER</t>
   </si>
   <si>
-    <t>P78E05-1000-CUI</t>
-  </si>
-  <si>
     <t>U9</t>
   </si>
   <si>
@@ -896,12 +884,21 @@
   </si>
   <si>
     <t>DATA 6/5/2024</t>
+  </si>
+  <si>
+    <t>DC/DC 9V 1A</t>
+  </si>
+  <si>
+    <t>M: 490-P78E09-1000</t>
+  </si>
+  <si>
+    <t>P78E09-1000-CUI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1494,9 +1491,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1534,7 +1531,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1640,7 +1637,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1782,18 +1779,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="J62" sqref="J62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1814,11 +1811,11 @@
   <sheetData>
     <row r="1" spans="1:11" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C1" s="5"/>
       <c r="G1" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -3618,7 +3615,7 @@
       </c>
       <c r="K56" s="8"/>
     </row>
-    <row r="57" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="8">
         <v>54</v>
       </c>
@@ -3761,25 +3758,25 @@
         <v>258</v>
       </c>
       <c r="D61" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="E61" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="E61" s="8" t="s">
+      <c r="F61" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="G61" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="H61" s="8" t="s">
         <v>260</v>
-      </c>
-      <c r="F61" s="8" t="s">
-        <v>261</v>
-      </c>
-      <c r="G61" s="8" t="s">
-        <v>262</v>
-      </c>
-      <c r="H61" s="8" t="s">
-        <v>263</v>
       </c>
       <c r="I61" s="8" t="s">
         <v>137</v>
       </c>
       <c r="J61" s="8" t="s">
-        <v>264</v>
+        <v>289</v>
       </c>
       <c r="K61" s="8" t="s">
         <v>250</v>
@@ -3793,28 +3790,28 @@
         <v>1</v>
       </c>
       <c r="C62" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="E62" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="F62" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="G62" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="H62" s="8" t="s">
         <v>265</v>
       </c>
-      <c r="D62" s="8" t="s">
+      <c r="I62" s="8" t="s">
         <v>266</v>
       </c>
-      <c r="E62" s="8" t="s">
+      <c r="J62" s="8" t="s">
         <v>267</v>
-      </c>
-      <c r="F62" s="8" t="s">
-        <v>267</v>
-      </c>
-      <c r="G62" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="H62" s="8" t="s">
-        <v>269</v>
-      </c>
-      <c r="I62" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="J62" s="8" t="s">
-        <v>271</v>
       </c>
       <c r="K62" s="8" t="s">
         <v>250</v>
@@ -3828,31 +3825,31 @@
         <v>1</v>
       </c>
       <c r="C63" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="E63" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="F63" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="G63" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="H63" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="D63" s="8" t="s">
+      <c r="I63" s="8" t="s">
         <v>273</v>
       </c>
-      <c r="E63" s="8" t="s">
+      <c r="J63" s="8" t="s">
         <v>274</v>
       </c>
-      <c r="F63" s="8" t="s">
-        <v>274</v>
-      </c>
-      <c r="G63" s="8" t="s">
+      <c r="K63" s="8" t="s">
         <v>275</v>
-      </c>
-      <c r="H63" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="I63" s="8" t="s">
-        <v>277</v>
-      </c>
-      <c r="J63" s="8" t="s">
-        <v>278</v>
-      </c>
-      <c r="K63" s="8" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="64" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -3863,31 +3860,31 @@
         <v>1</v>
       </c>
       <c r="C64" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="D64" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="E64" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="F64" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="G64" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="D64" s="8" t="s">
+      <c r="H64" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="E64" s="8" t="s">
+      <c r="I64" s="8" t="s">
         <v>282</v>
       </c>
-      <c r="F64" s="8" t="s">
+      <c r="J64" s="8" t="s">
         <v>283</v>
       </c>
-      <c r="G64" s="8" t="s">
+      <c r="K64" s="8" t="s">
         <v>284</v>
-      </c>
-      <c r="H64" s="8" t="s">
-        <v>285</v>
-      </c>
-      <c r="I64" s="8" t="s">
-        <v>286</v>
-      </c>
-      <c r="J64" s="8" t="s">
-        <v>287</v>
-      </c>
-      <c r="K64" s="8" t="s">
-        <v>288</v>
       </c>
     </row>
   </sheetData>

</xml_diff>